<commit_message>
almost ready for tabs
added more content. Went a little overboard but I needed something to work with
</commit_message>
<xml_diff>
--- a/resources/concatenator.xlsx
+++ b/resources/concatenator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwybo\Desktop\Midnight Monsters\GH\Midnight393-Website\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7BEB8E-C7AA-49FA-A144-73845C4A7932}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1884B239-2486-4D6C-A526-26F3785B353A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{4AABC04B-DC5D-4C5B-BFA6-E1508A2510C1}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="32">
   <si>
     <t>discord</t>
   </si>
@@ -101,6 +101,35 @@
   </si>
   <si>
     <t>&lt;/a&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lorem ipsum dolor amet tousled edison bulb activated charcoal biodiesel echo park 8-bit. Copper mug pickled keffiyeh, vice pork belly gluten-free lumbersexual bicycle rights succulents church-key gentrify. Put a bird on it intelligentsia ethical bitters squid DIY meh microdosing. Food truck seitan ramps man braid brunch pinterest biodiesel cardigan shoreditch shabby chic. Semiotics squid raclette, narwhal vinyl wolf cronut direct trade. Pug everyday carry irony, cold-pressed brunch portland cronut roof party echo park 3 wolf moon fingerstache craft beer authentic lyft.&lt;/p&gt;
+&lt;p&gt;Master cleanse mlkshk cliche, swag skateboard shoreditch farm-to-table. Single-origin coffee 90's organic bicycle rights tumblr literally selvage. Affogato lyft vinyl, vexillologist ramps chambray mumblecore semiotics snackwave. Palo santo ennui paleo chia, williamsburg 8-bit leggings ramps gochujang intelligentsia biodiesel iPhone tilde.&lt;/p&gt;
+&lt;p&gt;Messenger bag pinterest forage literally, lo-fi umami YOLO jean shorts cliche post-ironic. Migas banh mi tacos, poutine seitan drinking vinegar squid. Hammock bushwick tofu roof party, coloring book butcher umami kitsch hexagon pour-over shabby chic single-origin coffee iceland cronut shoreditch. Heirloom brunch kitsch next level ennui gochujang green juice meggings man braid trust fund hella selfies. Hexagon YOLO raclette stumptown migas, vape lo-fi banjo.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Need emergency pens and paper for an important meeting? Office Depot has your back.</t>
+  </si>
+  <si>
+    <t>With same-day in-store pickup, it's a bad day to be a business problem.</t>
+  </si>
+  <si>
+    <t>Come on down to Gerry Smith's rootin' tootin' Office Supply store</t>
+  </si>
+  <si>
+    <t>Top 21 reasons why Office Depot is better than staples</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;I don't know what to tell you it's just not.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Who's tryna play some fortnite comp nades only must be over 18 'cause we're using cuss words</t>
+  </si>
+  <si>
+    <t>Fuck I can't think of any good titles</t>
+  </si>
+  <si>
+    <t>Insert Title Here I guess</t>
   </si>
 </sst>
 </file>
@@ -124,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +163,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,11 +186,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -624,10 +663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B714D08-DFAB-4E3B-B3AA-30BED48F46EA}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,11 +674,13 @@
     <col min="1" max="1" width="39.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="94.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="69.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.88671875" style="5"/>
+    <col min="24" max="24" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -685,8 +726,41 @@
         <f>CONCATENATE(I1,J1,K1,L1,M1)</f>
         <v>&lt;li&gt;&lt;a href="#how_to_stay_woke_on_csgo"&gt;How to stay woke on CSGO&lt;/a&gt;&lt;/li&gt;</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="str">
+        <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(O1," ","_"),CHAR(39),""),CHAR(46),""))</f>
+        <v>need_emergency_pens_and_paper_for_an_important_meeting?_office_depot_has_your_back</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="str">
+        <f>O1</f>
+        <v>Need emergency pens and paper for an important meeting? Office Depot has your back.</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="5" t="str">
+        <f>CONCATENATE(P1,Q1,R1,S1,T1,U1)</f>
+        <v>&lt;h2 id="need_emergency_pens_and_paper_for_an_important_meeting?_office_depot_has_your_back"&gt;Need emergency pens and paper for an important meeting? Office Depot has your back.&lt;/h2&gt;&lt;p&gt;Lorem ipsum dolor amet tousled edison bulb activated charcoal biodiesel echo park 8-bit. Copper mug pickled keffiyeh, vice pork belly gluten-free lumbersexual bicycle rights succulents church-key gentrify. Put a bird on it intelligentsia ethical bitters squid DIY meh microdosing. Food truck seitan ramps man braid brunch pinterest biodiesel cardigan shoreditch shabby chic. Semiotics squid raclette, narwhal vinyl wolf cronut direct trade. Pug everyday carry irony, cold-pressed brunch portland cronut roof party echo park 3 wolf moon fingerstache craft beer authentic lyft.&lt;/p&gt;
+&lt;p&gt;Master cleanse mlkshk cliche, swag skateboard shoreditch farm-to-table. Single-origin coffee 90's organic bicycle rights tumblr literally selvage. Affogato lyft vinyl, vexillologist ramps chambray mumblecore semiotics snackwave. Palo santo ennui paleo chia, williamsburg 8-bit leggings ramps gochujang intelligentsia biodiesel iPhone tilde.&lt;/p&gt;
+&lt;p&gt;Messenger bag pinterest forage literally, lo-fi umami YOLO jean shorts cliche post-ironic. Migas banh mi tacos, poutine seitan drinking vinegar squid. Hammock bushwick tofu roof party, coloring book butcher umami kitsch hexagon pour-over shabby chic single-origin coffee iceland cronut shoreditch. Heirloom brunch kitsch next level ennui gochujang green juice meggings man braid trust fund hella selfies. Hexagon YOLO raclette stumptown migas, vape lo-fi banjo.&lt;/p&gt;</v>
+      </c>
+      <c r="X1" s="5" t="str">
+        <f>CONCATENATE(I1,Q1,K1,O1,M1)</f>
+        <v>&lt;li&gt;&lt;a href="#need_emergency_pens_and_paper_for_an_important_meeting?_office_depot_has_your_back"&gt;Need emergency pens and paper for an important meeting? Office Depot has your back.&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -732,8 +806,41 @@
         <f t="shared" ref="N2:N3" si="5">CONCATENATE(I2,J2,K2,L2,M2)</f>
         <v>&lt;li&gt;&lt;a href="#knives_only"&gt;Knives only&lt;/a&gt;&lt;/li&gt;</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q7" si="6">LOWER(SUBSTITUTE(SUBSTITUTE(O2," ","_"),CHAR(39),""))</f>
+        <v>with_same-day_in-store_pickup,_its_a_bad_day_to_be_a_business_problem.</v>
+      </c>
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" t="str">
+        <f t="shared" ref="S2:S7" si="7">O2</f>
+        <v>With same-day in-store pickup, it's a bad day to be a business problem.</v>
+      </c>
+      <c r="T2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" s="5" t="str">
+        <f t="shared" ref="V2:V7" si="8">CONCATENATE(P2,Q2,R2,S2,T2,U2)</f>
+        <v>&lt;h2 id="with_same-day_in-store_pickup,_its_a_bad_day_to_be_a_business_problem."&gt;With same-day in-store pickup, it's a bad day to be a business problem.&lt;/h2&gt;&lt;p&gt;Lorem ipsum dolor amet tousled edison bulb activated charcoal biodiesel echo park 8-bit. Copper mug pickled keffiyeh, vice pork belly gluten-free lumbersexual bicycle rights succulents church-key gentrify. Put a bird on it intelligentsia ethical bitters squid DIY meh microdosing. Food truck seitan ramps man braid brunch pinterest biodiesel cardigan shoreditch shabby chic. Semiotics squid raclette, narwhal vinyl wolf cronut direct trade. Pug everyday carry irony, cold-pressed brunch portland cronut roof party echo park 3 wolf moon fingerstache craft beer authentic lyft.&lt;/p&gt;
+&lt;p&gt;Master cleanse mlkshk cliche, swag skateboard shoreditch farm-to-table. Single-origin coffee 90's organic bicycle rights tumblr literally selvage. Affogato lyft vinyl, vexillologist ramps chambray mumblecore semiotics snackwave. Palo santo ennui paleo chia, williamsburg 8-bit leggings ramps gochujang intelligentsia biodiesel iPhone tilde.&lt;/p&gt;
+&lt;p&gt;Messenger bag pinterest forage literally, lo-fi umami YOLO jean shorts cliche post-ironic. Migas banh mi tacos, poutine seitan drinking vinegar squid. Hammock bushwick tofu roof party, coloring book butcher umami kitsch hexagon pour-over shabby chic single-origin coffee iceland cronut shoreditch. Heirloom brunch kitsch next level ennui gochujang green juice meggings man braid trust fund hella selfies. Hexagon YOLO raclette stumptown migas, vape lo-fi banjo.&lt;/p&gt;</v>
+      </c>
+      <c r="X2" s="5" t="str">
+        <f t="shared" ref="X2:X7" si="9">CONCATENATE(I2,Q2,K2,O2,M2)</f>
+        <v>&lt;li&gt;&lt;a href="#with_same-day_in-store_pickup,_its_a_bad_day_to_be_a_business_problem."&gt;With same-day in-store pickup, it's a bad day to be a business problem.&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -779,9 +886,258 @@
         <f t="shared" si="5"/>
         <v>&lt;li&gt;&lt;a href="#how_to_keep_track_of_whos_fucking_your_mom"&gt;How to keep track of who's fucking your mom&lt;/a&gt;&lt;/li&gt;</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" si="6"/>
+        <v>come_on_down_to_gerry_smiths_rootin_tootin_office_supply_store</v>
+      </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" t="str">
+        <f t="shared" si="7"/>
+        <v>Come on down to Gerry Smith's rootin' tootin' Office Supply store</v>
+      </c>
+      <c r="T3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>&lt;h2 id="come_on_down_to_gerry_smiths_rootin_tootin_office_supply_store"&gt;Come on down to Gerry Smith's rootin' tootin' Office Supply store&lt;/h2&gt;&lt;p&gt;Lorem ipsum dolor amet tousled edison bulb activated charcoal biodiesel echo park 8-bit. Copper mug pickled keffiyeh, vice pork belly gluten-free lumbersexual bicycle rights succulents church-key gentrify. Put a bird on it intelligentsia ethical bitters squid DIY meh microdosing. Food truck seitan ramps man braid brunch pinterest biodiesel cardigan shoreditch shabby chic. Semiotics squid raclette, narwhal vinyl wolf cronut direct trade. Pug everyday carry irony, cold-pressed brunch portland cronut roof party echo park 3 wolf moon fingerstache craft beer authentic lyft.&lt;/p&gt;
+&lt;p&gt;Master cleanse mlkshk cliche, swag skateboard shoreditch farm-to-table. Single-origin coffee 90's organic bicycle rights tumblr literally selvage. Affogato lyft vinyl, vexillologist ramps chambray mumblecore semiotics snackwave. Palo santo ennui paleo chia, williamsburg 8-bit leggings ramps gochujang intelligentsia biodiesel iPhone tilde.&lt;/p&gt;
+&lt;p&gt;Messenger bag pinterest forage literally, lo-fi umami YOLO jean shorts cliche post-ironic. Migas banh mi tacos, poutine seitan drinking vinegar squid. Hammock bushwick tofu roof party, coloring book butcher umami kitsch hexagon pour-over shabby chic single-origin coffee iceland cronut shoreditch. Heirloom brunch kitsch next level ennui gochujang green juice meggings man braid trust fund hella selfies. Hexagon YOLO raclette stumptown migas, vape lo-fi banjo.&lt;/p&gt;</v>
+      </c>
+      <c r="X3" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;li&gt;&lt;a href="#come_on_down_to_gerry_smiths_rootin_tootin_office_supply_store"&gt;Come on down to Gerry Smith's rootin' tootin' Office Supply store&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="6"/>
+        <v>top_21_reasons_why_office_depot_is_better_than_staples</v>
+      </c>
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="7"/>
+        <v>Top 21 reasons why Office Depot is better than staples</v>
+      </c>
+      <c r="T4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V4" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>&lt;h2 id="top_21_reasons_why_office_depot_is_better_than_staples"&gt;Top 21 reasons why Office Depot is better than staples&lt;/h2&gt;&lt;p&gt;I don't know what to tell you it's just not.&lt;/p&gt;</v>
+      </c>
+      <c r="X4" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;li&gt;&lt;a href="#top_21_reasons_why_office_depot_is_better_than_staples"&gt;Top 21 reasons why Office Depot is better than staples&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="6"/>
+        <v>whos_tryna_play_some_fortnite_comp_nades_only_must_be_over_18_cause_were_using_cuss_words</v>
+      </c>
+      <c r="R5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" si="7"/>
+        <v>Who's tryna play some fortnite comp nades only must be over 18 'cause we're using cuss words</v>
+      </c>
+      <c r="T5" t="s">
+        <v>18</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V5" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>&lt;h2 id="whos_tryna_play_some_fortnite_comp_nades_only_must_be_over_18_cause_were_using_cuss_words"&gt;Who's tryna play some fortnite comp nades only must be over 18 'cause we're using cuss words&lt;/h2&gt;&lt;p&gt;Lorem ipsum dolor amet tousled edison bulb activated charcoal biodiesel echo park 8-bit. Copper mug pickled keffiyeh, vice pork belly gluten-free lumbersexual bicycle rights succulents church-key gentrify. Put a bird on it intelligentsia ethical bitters squid DIY meh microdosing. Food truck seitan ramps man braid brunch pinterest biodiesel cardigan shoreditch shabby chic. Semiotics squid raclette, narwhal vinyl wolf cronut direct trade. Pug everyday carry irony, cold-pressed brunch portland cronut roof party echo park 3 wolf moon fingerstache craft beer authentic lyft.&lt;/p&gt;
+&lt;p&gt;Master cleanse mlkshk cliche, swag skateboard shoreditch farm-to-table. Single-origin coffee 90's organic bicycle rights tumblr literally selvage. Affogato lyft vinyl, vexillologist ramps chambray mumblecore semiotics snackwave. Palo santo ennui paleo chia, williamsburg 8-bit leggings ramps gochujang intelligentsia biodiesel iPhone tilde.&lt;/p&gt;
+&lt;p&gt;Messenger bag pinterest forage literally, lo-fi umami YOLO jean shorts cliche post-ironic. Migas banh mi tacos, poutine seitan drinking vinegar squid. Hammock bushwick tofu roof party, coloring book butcher umami kitsch hexagon pour-over shabby chic single-origin coffee iceland cronut shoreditch. Heirloom brunch kitsch next level ennui gochujang green juice meggings man braid trust fund hella selfies. Hexagon YOLO raclette stumptown migas, vape lo-fi banjo.&lt;/p&gt;</v>
+      </c>
+      <c r="X5" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;li&gt;&lt;a href="#whos_tryna_play_some_fortnite_comp_nades_only_must_be_over_18_cause_were_using_cuss_words"&gt;Who's tryna play some fortnite comp nades only must be over 18 'cause we're using cuss words&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="6"/>
+        <v>fuck_i_cant_think_of_any_good_titles</v>
+      </c>
+      <c r="R6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="7"/>
+        <v>Fuck I can't think of any good titles</v>
+      </c>
+      <c r="T6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>&lt;h2 id="fuck_i_cant_think_of_any_good_titles"&gt;Fuck I can't think of any good titles&lt;/h2&gt;&lt;p&gt;Lorem ipsum dolor amet tousled edison bulb activated charcoal biodiesel echo park 8-bit. Copper mug pickled keffiyeh, vice pork belly gluten-free lumbersexual bicycle rights succulents church-key gentrify. Put a bird on it intelligentsia ethical bitters squid DIY meh microdosing. Food truck seitan ramps man braid brunch pinterest biodiesel cardigan shoreditch shabby chic. Semiotics squid raclette, narwhal vinyl wolf cronut direct trade. Pug everyday carry irony, cold-pressed brunch portland cronut roof party echo park 3 wolf moon fingerstache craft beer authentic lyft.&lt;/p&gt;
+&lt;p&gt;Master cleanse mlkshk cliche, swag skateboard shoreditch farm-to-table. Single-origin coffee 90's organic bicycle rights tumblr literally selvage. Affogato lyft vinyl, vexillologist ramps chambray mumblecore semiotics snackwave. Palo santo ennui paleo chia, williamsburg 8-bit leggings ramps gochujang intelligentsia biodiesel iPhone tilde.&lt;/p&gt;
+&lt;p&gt;Messenger bag pinterest forage literally, lo-fi umami YOLO jean shorts cliche post-ironic. Migas banh mi tacos, poutine seitan drinking vinegar squid. Hammock bushwick tofu roof party, coloring book butcher umami kitsch hexagon pour-over shabby chic single-origin coffee iceland cronut shoreditch. Heirloom brunch kitsch next level ennui gochujang green juice meggings man braid trust fund hella selfies. Hexagon YOLO raclette stumptown migas, vape lo-fi banjo.&lt;/p&gt;</v>
+      </c>
+      <c r="X6" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;li&gt;&lt;a href="#fuck_i_cant_think_of_any_good_titles"&gt;Fuck I can't think of any good titles&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="6"/>
+        <v>insert_title_here_i_guess</v>
+      </c>
+      <c r="R7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="7"/>
+        <v>Insert Title Here I guess</v>
+      </c>
+      <c r="T7" t="s">
+        <v>18</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V7" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>&lt;h2 id="insert_title_here_i_guess"&gt;Insert Title Here I guess&lt;/h2&gt;&lt;p&gt;Lorem ipsum dolor amet tousled edison bulb activated charcoal biodiesel echo park 8-bit. Copper mug pickled keffiyeh, vice pork belly gluten-free lumbersexual bicycle rights succulents church-key gentrify. Put a bird on it intelligentsia ethical bitters squid DIY meh microdosing. Food truck seitan ramps man braid brunch pinterest biodiesel cardigan shoreditch shabby chic. Semiotics squid raclette, narwhal vinyl wolf cronut direct trade. Pug everyday carry irony, cold-pressed brunch portland cronut roof party echo park 3 wolf moon fingerstache craft beer authentic lyft.&lt;/p&gt;
+&lt;p&gt;Master cleanse mlkshk cliche, swag skateboard shoreditch farm-to-table. Single-origin coffee 90's organic bicycle rights tumblr literally selvage. Affogato lyft vinyl, vexillologist ramps chambray mumblecore semiotics snackwave. Palo santo ennui paleo chia, williamsburg 8-bit leggings ramps gochujang intelligentsia biodiesel iPhone tilde.&lt;/p&gt;
+&lt;p&gt;Messenger bag pinterest forage literally, lo-fi umami YOLO jean shorts cliche post-ironic. Migas banh mi tacos, poutine seitan drinking vinegar squid. Hammock bushwick tofu roof party, coloring book butcher umami kitsch hexagon pour-over shabby chic single-origin coffee iceland cronut shoreditch. Heirloom brunch kitsch next level ennui gochujang green juice meggings man braid trust fund hella selfies. Hexagon YOLO raclette stumptown migas, vape lo-fi banjo.&lt;/p&gt;</v>
+      </c>
+      <c r="X7" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;li&gt;&lt;a href="#insert_title_here_i_guess"&gt;Insert Title Here I guess&lt;/a&gt;&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>